<commit_message>
Fixed the null error in apache!
</commit_message>
<xml_diff>
--- a/UserSchedules.xlsx
+++ b/UserSchedules.xlsx
@@ -14,8 +14,8 @@
   </bookViews>
   <sheets>
     <sheet name="Test2" sheetId="4" r:id="rId2"/>
-    <sheet name="testing" r:id="rId8" sheetId="5"/>
     <sheet name="Kat" r:id="rId9" sheetId="6"/>
+    <sheet name="testing" r:id="rId8" sheetId="7"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
   <si>
     <t>MATH 101</t>
   </si>
@@ -459,45 +459,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H2"/>
@@ -561,4 +522,43 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Comments and trying to do the add a recreate from log system.
</commit_message>
<xml_diff>
--- a/UserSchedules.xlsx
+++ b/UserSchedules.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Test2" sheetId="4" r:id="rId2"/>
     <sheet name="Kat" r:id="rId9" sheetId="6"/>
     <sheet name="testing" r:id="rId8" sheetId="7"/>
+    <sheet name="za" r:id="rId10" sheetId="8"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="27">
   <si>
     <t>MATH 101</t>
   </si>
@@ -97,6 +98,27 @@
   </si>
   <si>
     <t>304</t>
+  </si>
+  <si>
+    <t>COMP 220  A</t>
+  </si>
+  <si>
+    <t>COMP PROGRAMMIN</t>
+  </si>
+  <si>
+    <t>COMP PROGRAMMING II</t>
+  </si>
+  <si>
+    <t>9:00:00</t>
+  </si>
+  <si>
+    <t>9:50:00</t>
+  </si>
+  <si>
+    <t>STEM</t>
+  </si>
+  <si>
+    <t>326</t>
   </si>
 </sst>
 </file>
@@ -561,4 +583,43 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Saving schedule in FXMain
</commit_message>
<xml_diff>
--- a/UserSchedules.xlsx
+++ b/UserSchedules.xlsx
@@ -17,6 +17,7 @@
     <sheet name="Kat" r:id="rId9" sheetId="6"/>
     <sheet name="testing" r:id="rId8" sheetId="7"/>
     <sheet name="za" r:id="rId10" sheetId="8"/>
+    <sheet name="cheese" r:id="rId11" sheetId="9"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="41">
   <si>
     <t>MATH 101</t>
   </si>
@@ -119,6 +120,48 @@
   </si>
   <si>
     <t>326</t>
+  </si>
+  <si>
+    <t>COMP 222  B</t>
+  </si>
+  <si>
+    <t>DATA STRUC/ALGO</t>
+  </si>
+  <si>
+    <t>INTRO TO DATA STRUCT &amp; ALGORITHMS</t>
+  </si>
+  <si>
+    <t>11:30:00</t>
+  </si>
+  <si>
+    <t>12:45:00</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>376</t>
+  </si>
+  <si>
+    <t>EDUC 312  A</t>
+  </si>
+  <si>
+    <t>MUSIC METHODS</t>
+  </si>
+  <si>
+    <t>SECONDARY MUSIC METH-MUS ED MAJ</t>
+  </si>
+  <si>
+    <t>10:05:00</t>
+  </si>
+  <si>
+    <t>11:20:00</t>
+  </si>
+  <si>
+    <t>PFAC</t>
+  </si>
+  <si>
+    <t>68</t>
   </si>
 </sst>
 </file>
@@ -622,4 +665,69 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>